<commit_message>
CSYS Added & STDG/INT2 files rearranged.
</commit_message>
<xml_diff>
--- a/output/CSYS_2000.xlsx
+++ b/output/CSYS_2000.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -496,7 +496,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -519,7 +519,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -542,7 +542,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -565,7 +565,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -588,7 +588,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -611,7 +611,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -634,7 +634,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -657,7 +657,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -680,7 +680,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -703,7 +703,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -726,7 +726,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -749,7 +749,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -772,7 +772,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -795,7 +795,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -818,7 +818,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -841,7 +841,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -864,7 +864,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -887,7 +887,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -910,7 +910,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -933,7 +933,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -956,7 +956,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -979,7 +979,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1002,7 +1002,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1025,7 +1025,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1048,7 +1048,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1071,7 +1071,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1094,7 +1094,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1117,7 +1117,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1186,7 +1186,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1209,7 +1209,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1232,7 +1232,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -1255,7 +1255,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1278,7 +1278,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1324,7 +1324,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1370,7 +1370,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1416,7 +1416,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -1462,7 +1462,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -1508,7 +1508,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -1531,7 +1531,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -1554,7 +1554,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -1577,7 +1577,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1600,7 +1600,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1623,7 +1623,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -1646,7 +1646,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1669,7 +1669,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1692,7 +1692,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -1715,7 +1715,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D57" t="n">

</xml_diff>